<commit_message>
Fix issue with ficha variable initialization
</commit_message>
<xml_diff>
--- a/static/schedule-courses/Horario 1-2024 - 2693180.xlsx
+++ b/static/schedule-courses/Horario 1-2024 - 2693180.xlsx
@@ -517,6 +517,16 @@
           <t>2693180</t>
         </is>
       </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>Instructor titular:</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>BERNARDO ZAPATA BAENA</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -656,36 +666,36 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>nan 
- YORMAN ANDRÉS CALDERÓN YEPES 
+          <t>INGLES 
+ NUEVO INGLÉS 
  504</t>
         </is>
       </c>
@@ -699,36 +709,36 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>nan 
- YORMAN ANDRÉS CALDERÓN YEPES 
+          <t>INGLES 
+ NUEVO INGLÉS 
  504</t>
         </is>
       </c>
@@ -742,35 +752,35 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
@@ -785,35 +795,35 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
@@ -828,35 +838,35 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
@@ -871,35 +881,35 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>nan 
+          <t>CONFIGURACION DE SERVICIOS 
  BERNARDO ZAPATA BAENA 
  504</t>
         </is>

</xml_diff>